<commit_message>
Added: Addeding Signup feacture of this  project
</commit_message>
<xml_diff>
--- a/src/main/java/com/KeywordDriven/scenarios/hubspot.xlsx
+++ b/src/main/java/com/KeywordDriven/scenarios/hubspot.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\KeyWordDrivenFramwork\src\main\java\com\KeywordDriven\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82E862E-B8CE-4926-B18E-CBF9025C3D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C011A557-0B41-404E-AE08-0017BC69B4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{919DEB6C-C893-4C12-8550-4BA5A847B583}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="signUp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>test steps</t>
   </si>
@@ -117,13 +118,22 @@
   </si>
   <si>
     <t>Sign up</t>
+  </si>
+  <si>
+    <t>test step</t>
+  </si>
+  <si>
+    <t>http://app.hubspot.com/login</t>
+  </si>
+  <si>
+    <t>quit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +149,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -163,18 +222,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{1FEDBC62-6A2D-49C8-BD9A-988EAD1498A8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{7E95A3F5-8098-47AC-A079-4DFBCC0ECA41}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -695,4 +762,114 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6825BE61-1FE6-4E17-9DE4-A50B34E7A437}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>